<commit_message>
Refactor init product detail page for another test
</commit_message>
<xml_diff>
--- a/src/main/resources/excels/check_product_detail_sf/BH_8616_Check hide remaining stock on online store.xlsx
+++ b/src/main/resources/excels/check_product_detail_sf/BH_8616_Check hide remaining stock on online store.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Auto\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -161,11 +161,18 @@
     - Branch name
     - Buy now, Add to cart...</t>
   </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -517,11 +524,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" customWidth="1"/>
-    <col min="3" max="3" width="58.33203125" customWidth="1"/>
-    <col min="4" max="4" width="38.88671875" customWidth="1"/>
-    <col min="5" max="5" width="54.109375" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="58.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="38.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="54.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -560,7 +567,9 @@
       <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="114" x14ac:dyDescent="0.25">
@@ -579,7 +588,9 @@
       <c r="E3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="114" x14ac:dyDescent="0.25">
@@ -598,7 +609,9 @@
       <c r="E4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="114" x14ac:dyDescent="0.25">
@@ -617,7 +630,9 @@
       <c r="E5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="114" x14ac:dyDescent="0.25">
@@ -636,7 +651,9 @@
       <c r="E6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="114" x14ac:dyDescent="0.25">
@@ -655,7 +672,9 @@
       <c r="E7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="10"/>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="114" x14ac:dyDescent="0.25">
@@ -674,7 +693,9 @@
       <c r="E8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="10"/>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="114" x14ac:dyDescent="0.25">
@@ -693,7 +714,9 @@
       <c r="E9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="10"/>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="114" x14ac:dyDescent="0.25">
@@ -712,7 +735,9 @@
       <c r="E10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="12"/>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="114" x14ac:dyDescent="0.25">
@@ -731,7 +756,9 @@
       <c r="E11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="12"/>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="114" x14ac:dyDescent="0.25">
@@ -750,7 +777,9 @@
       <c r="E12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="12"/>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="114" x14ac:dyDescent="0.25">
@@ -769,7 +798,9 @@
       <c r="E13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="12"/>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Product detail] Fix check price and discount badge
</commit_message>
<xml_diff>
--- a/src/main/resources/excels/check_product_detail_sf/BH_8616_Check hide remaining stock on online store.xlsx
+++ b/src/main/resources/excels/check_product_detail_sf/BH_8616_Check hide remaining stock on online store.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\IdeaProjects\GoSELL-Automation\src\main\resources\excels\check_product_detail_sf\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="38">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -161,11 +161,18 @@
     - Branch name
     - Buy now, Add to cart...</t>
   </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -517,11 +524,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="58.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="54.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="58.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="38.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="54.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -560,6 +567,9 @@
       <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
@@ -578,6 +588,9 @@
       <c r="E3" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
@@ -596,6 +609,9 @@
       <c r="E4" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
@@ -614,6 +630,9 @@
       <c r="E5" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
@@ -632,6 +651,9 @@
       <c r="E6" s="10" t="s">
         <v>18</v>
       </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
@@ -650,6 +672,9 @@
       <c r="E7" s="10" t="s">
         <v>18</v>
       </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
@@ -668,6 +693,9 @@
       <c r="E8" s="10" t="s">
         <v>18</v>
       </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
@@ -686,6 +714,9 @@
       <c r="E9" s="10" t="s">
         <v>18</v>
       </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
@@ -704,6 +735,9 @@
       <c r="E10" s="12" t="s">
         <v>18</v>
       </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
@@ -722,6 +756,9 @@
       <c r="E11" s="12" t="s">
         <v>18</v>
       </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
@@ -740,6 +777,9 @@
       <c r="E12" s="12" t="s">
         <v>18</v>
       </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
@@ -757,6 +797,9 @@
       </c>
       <c r="E13" s="12" t="s">
         <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
       </c>
       <c r="G13" s="2"/>
     </row>

</xml_diff>

<commit_message>
1. Add parameter for test config 2. Add create/update supplier testcase 3. Commit task: BH-21331,BH-21332,BH-21333,BH-21334
</commit_message>
<xml_diff>
--- a/src/main/resources/excels/check_product_detail_sf/BH_8616_Check hide remaining stock on online store.xlsx
+++ b/src/main/resources/excels/check_product_detail_sf/BH_8616_Check hide remaining stock on online store.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="38">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -652,7 +652,7 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -673,7 +673,7 @@
         <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -694,7 +694,7 @@
         <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -715,7 +715,7 @@
         <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9" s="2"/>
     </row>
@@ -757,7 +757,7 @@
         <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11" s="2"/>
     </row>
@@ -778,7 +778,7 @@
         <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G12" s="2"/>
     </row>
@@ -799,7 +799,7 @@
         <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" s="2"/>
     </row>

</xml_diff>

<commit_message>
Refactor code for run config
</commit_message>
<xml_diff>
--- a/src/main/resources/excels/check_product_detail_sf/BH_8616_Check hide remaining stock on online store.xlsx
+++ b/src/main/resources/excels/check_product_detail_sf/BH_8616_Check hide remaining stock on online store.xlsx
@@ -3,24 +3,27 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\IdeaProjects\GoSELL-Automation\src\main\resources\excels\check_product_detail_sf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8008C7FB-A735-40A0-B1A0-C1D64F546B46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B4D08B-4CDE-4E2E-B1F1-490F1298D880}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$13</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="39">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -32,9 +35,6 @@
   </si>
   <si>
     <t>Expected</t>
-  </si>
-  <si>
-    <t>Result</t>
   </si>
   <si>
     <t>BH_8616_G1_Case1_1</t>
@@ -167,12 +167,17 @@
   <si>
     <t>PASS</t>
   </si>
+  <si>
+    <t>Result VIE</t>
+  </si>
+  <si>
+    <t>Result ENG</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -264,13 +269,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -524,284 +526,311 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="58.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="38.88671875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="54.109375" collapsed="true"/>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="58.33203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="38.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="54.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="C4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="G6" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="8" t="s">
+    </row>
+    <row r="7" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="C7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="C8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="10" t="s">
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="C10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="10" t="s">
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="C12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="10" t="s">
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="10" t="s">
+      <c r="C13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="G13" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="102.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>

</xml_diff>

<commit_message>
Commit task: BH-21335, BH-21336, BH-21337
</commit_message>
<xml_diff>
--- a/src/main/resources/excels/check_product_detail_sf/BH_8616_Check hide remaining stock on online store.xlsx
+++ b/src/main/resources/excels/check_product_detail_sf/BH_8616_Check hide remaining stock on online store.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\IdeaProjects\GoSELL-Automation\src\main\resources\excels\check_product_detail_sf\"/>
     </mc:Choice>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="39">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -178,6 +178,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -526,11 +527,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="58.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="54.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="58.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="38.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="54.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -757,7 +758,7 @@
         <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
fix bugs not get the latest branch status
</commit_message>
<xml_diff>
--- a/src/main/resources/excels/check_product_detail_sf/BH_8616_Check hide remaining stock on online store.xlsx
+++ b/src/main/resources/excels/check_product_detail_sf/BH_8616_Check hide remaining stock on online store.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="39">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -666,7 +666,7 @@
         <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
         <v>35</v>
@@ -689,7 +689,7 @@
         <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s">
         <v>35</v>
@@ -712,7 +712,7 @@
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G8" t="s">
         <v>35</v>
@@ -735,7 +735,7 @@
         <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
         <v>35</v>
@@ -758,7 +758,7 @@
         <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G10" t="s">
         <v>36</v>
@@ -781,7 +781,7 @@
         <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G11" t="s">
         <v>35</v>
@@ -804,7 +804,7 @@
         <v>17</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G12" t="s">
         <v>35</v>
@@ -827,7 +827,7 @@
         <v>17</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G13" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Add script migrate tax rate, commission type for V-LIVE
</commit_message>
<xml_diff>
--- a/src/main/resources/excels/check_product_detail_sf/BH_8616_Check hide remaining stock on online store.xlsx
+++ b/src/main/resources/excels/check_product_detail_sf/BH_8616_Check hide remaining stock on online store.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="39">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -574,7 +574,7 @@
         <v>17</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>36</v>
@@ -666,7 +666,7 @@
         <v>17</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s" s="0">
         <v>35</v>
@@ -689,7 +689,7 @@
         <v>17</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s" s="0">
         <v>35</v>
@@ -712,7 +712,7 @@
         <v>17</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s" s="0">
         <v>35</v>
@@ -735,7 +735,7 @@
         <v>17</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s" s="0">
         <v>35</v>
@@ -758,7 +758,7 @@
         <v>17</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s" s="0">
         <v>36</v>
@@ -781,7 +781,7 @@
         <v>17</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s" s="0">
         <v>35</v>
@@ -804,7 +804,7 @@
         <v>17</v>
       </c>
       <c r="F12" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G12" t="s" s="0">
         <v>35</v>
@@ -827,7 +827,7 @@
         <v>17</v>
       </c>
       <c r="F13" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s" s="0">
         <v>35</v>

</xml_diff>